<commit_message>
Updated the dashboard file
</commit_message>
<xml_diff>
--- a/Crypto/doc/Dashboard.xlsx
+++ b/Crypto/doc/Dashboard.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="28120" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Multiplication</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Mouhamad</t>
+  </si>
+  <si>
+    <t>Rayan</t>
   </si>
 </sst>
 </file>
@@ -103,15 +109,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,15 +137,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -135,38 +170,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -537,7 +563,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -571,98 +597,112 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
@@ -683,19 +723,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="notContainsText" dxfId="5" priority="3" operator="notContains" text="x">
+    <cfRule type="notContainsText" dxfId="3" priority="3" operator="notContains" text="x">
       <formula>ISERROR(SEARCH("x",C2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="x">
+    <cfRule type="notContainsText" dxfId="0" priority="1" operator="notContains" text="x">
+      <formula>ISERROR(SEARCH("x",D2))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
-    </cfRule>
-    <cfRule type="notContainsText" dxfId="2" priority="1" operator="notContains" text="x">
-      <formula>ISERROR(SEARCH("x",D2))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>